<commit_message>
add support for keyed table
</commit_message>
<xml_diff>
--- a/tmp.xlsx
+++ b/tmp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\fsharp\qxl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D35A16-46AE-4550-B0DA-AED74E72CF64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C63CE5-5E18-49D7-865E-972C5F72758D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7980" yWindow="5415" windowWidth="23610" windowHeight="12645" xr2:uid="{925F285A-02D9-4967-A7DB-B6894CF61D1D}"/>
+    <workbookView xWindow="-25740" yWindow="1650" windowWidth="23610" windowHeight="12645" xr2:uid="{925F285A-02D9-4967-A7DB-B6894CF61D1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>uid</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>kimura</t>
+  </si>
+  <si>
+    <t>flip([]a:1 2 3;b: 4 5 6)</t>
+  </si>
+  <si>
+    <t>`a`b!(1 2; 3 4 5)</t>
+  </si>
+  <si>
+    <t>2!([]a:1 2 3;b: 4 5 6;c:5 6 7)</t>
   </si>
 </sst>
 </file>
@@ -436,39 +445,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531870C5-C8CB-45D0-A7B9-072551DB5602}">
-  <dimension ref="B3:C8"/>
+  <dimension ref="B3:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="H4" t="str" cm="1">
+        <f t="array" ref="H4:K5">_xll.dna_execute($C$10,$C$8,H3)</f>
+        <v>a</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+      <c r="M4" t="str" cm="1">
+        <f t="array" ref="M4:P5">_xll.dna_execute($C$10,$C$8,M3)</f>
+        <v>a</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="P4" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>8888</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+        <v>8866</v>
+      </c>
+      <c r="H5" t="str">
+        <v>b</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>6</v>
+      </c>
+      <c r="M5" t="str">
+        <v>b</v>
+      </c>
+      <c r="N5">
+        <v>3</v>
+      </c>
+      <c r="O5">
+        <v>4</v>
+      </c>
+      <c r="P5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -476,7 +541,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -484,13 +549,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="str" cm="1">
         <f t="array" ref="C8">_xll.dna_open_connection(C3,C4,C5,C6,C7)</f>
         <v>tmp</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E11" t="e" cm="1">
+        <f t="array" ref="E11">_xll.dna_execute($C$10,$C$8,E10)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add try exception when connecting to kdb
</commit_message>
<xml_diff>
--- a/tmp.xlsx
+++ b/tmp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\fsharp\qxl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C63CE5-5E18-49D7-865E-972C5F72758D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED889361-EB3B-48A7-AA0F-783F6AE96A81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25740" yWindow="1650" windowWidth="23610" windowHeight="12645" xr2:uid="{925F285A-02D9-4967-A7DB-B6894CF61D1D}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -93,7 +94,7 @@
     <t>`a`b!(1 2; 3 4 5)</t>
   </si>
   <si>
-    <t>2!([]a:1 2 3;b: 4 5 6;c:5 6 7)</t>
+    <t>1!([]a:1 2 3;b: 4 5 6;c:5 6 7)</t>
   </si>
 </sst>
 </file>
@@ -445,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531870C5-C8CB-45D0-A7B9-072551DB5602}">
-  <dimension ref="B3:P11"/>
+  <dimension ref="B3:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,9 +565,48 @@
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E11" t="e" cm="1">
-        <f t="array" ref="E11">_xll.dna_execute($C$10,$C$8,E10)</f>
-        <v>#VALUE!</v>
+      <c r="E11" t="str" cm="1">
+        <f t="array" ref="E11:G14">_xll.dna_execute($C$10,$C$8,E10)</f>
+        <v>a</v>
+      </c>
+      <c r="F11" t="str">
+        <v>b</v>
+      </c>
+      <c r="G11" t="str">
+        <v>c</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>6</v>
+      </c>
+      <c r="G14">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
char array to string to obj
</commit_message>
<xml_diff>
--- a/tmp.xlsx
+++ b/tmp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\fsharp\qxl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED889361-EB3B-48A7-AA0F-783F6AE96A81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DEFAEDB-3115-4CBC-BE05-FA1BEC9EA883}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25740" yWindow="1650" windowWidth="23610" windowHeight="12645" xr2:uid="{925F285A-02D9-4967-A7DB-B6894CF61D1D}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -56,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>uid</t>
   </si>
@@ -88,13 +87,7 @@
     <t>kimura</t>
   </si>
   <si>
-    <t>flip([]a:1 2 3;b: 4 5 6)</t>
-  </si>
-  <si>
-    <t>`a`b!(1 2; 3 4 5)</t>
-  </si>
-  <si>
-    <t>1!([]a:1 2 3;b: 4 5 6;c:5 6 7)</t>
+    <t>.sys 1</t>
   </si>
 </sst>
 </file>
@@ -446,111 +439,146 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531870C5-C8CB-45D0-A7B9-072551DB5602}">
-  <dimension ref="B3:P14"/>
+  <dimension ref="B3:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="44.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="H3" t="s">
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="M3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="H4" t="str" cm="1">
-        <f t="array" ref="H4:K5">_xll.dna_execute($C$10,$C$8,H3)</f>
-        <v>a</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>2</v>
-      </c>
-      <c r="K4">
-        <v>3</v>
-      </c>
-      <c r="M4" t="str" cm="1">
-        <f t="array" ref="M4:P5">_xll.dna_execute($C$10,$C$8,M3)</f>
-        <v>a</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="O4">
-        <v>2</v>
-      </c>
-      <c r="P4" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E4" t="str" cm="1">
+        <f t="array" ref="E4:K26">_xll.dna_execute($C$10,$C$8,E3)</f>
+        <v>folder</v>
+      </c>
+      <c r="F4" t="str">
+        <v>plant</v>
+      </c>
+      <c r="G4" t="str">
+        <v/>
+      </c>
+      <c r="H4" t="str">
+        <v/>
+      </c>
+      <c r="I4" t="str">
+        <v/>
+      </c>
+      <c r="J4" t="str">
+        <v/>
+      </c>
+      <c r="K4" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>8866</v>
+        <v>22002</v>
+      </c>
+      <c r="E5" t="str">
+        <v>env</v>
+      </c>
+      <c r="F5" t="str">
+        <v>deepData</v>
+      </c>
+      <c r="G5" t="str">
+        <v/>
       </c>
       <c r="H5" t="str">
-        <v>b</v>
-      </c>
-      <c r="I5">
-        <v>4</v>
-      </c>
-      <c r="J5">
-        <v>5</v>
-      </c>
-      <c r="K5">
-        <v>6</v>
-      </c>
-      <c r="M5" t="str">
-        <v>b</v>
-      </c>
-      <c r="N5">
-        <v>3</v>
-      </c>
-      <c r="O5">
-        <v>4</v>
-      </c>
-      <c r="P5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+      <c r="I5" t="str">
+        <v/>
+      </c>
+      <c r="J5" t="str">
+        <v/>
+      </c>
+      <c r="K5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E6" t="str">
+        <v>subsys</v>
+      </c>
+      <c r="F6" t="str">
+        <v>mxnet</v>
+      </c>
+      <c r="G6" t="str">
+        <v/>
+      </c>
+      <c r="H6" t="str">
+        <v/>
+      </c>
+      <c r="I6" t="str">
+        <v/>
+      </c>
+      <c r="J6" t="str">
+        <v/>
+      </c>
+      <c r="K6" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E7" t="str">
+        <v>process</v>
+      </c>
+      <c r="F7" t="str">
+        <v>cdb</v>
+      </c>
+      <c r="G7" t="str">
+        <v/>
+      </c>
+      <c r="H7" t="str">
+        <v/>
+      </c>
+      <c r="I7" t="str">
+        <v/>
+      </c>
+      <c r="J7" t="str">
+        <v/>
+      </c>
+      <c r="K7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -558,55 +586,440 @@
         <f t="array" ref="C8">_xll.dna_open_connection(C3,C4,C5,C6,C7)</f>
         <v>tmp</v>
       </c>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E11" t="str" cm="1">
-        <f t="array" ref="E11:G14">_xll.dna_execute($C$10,$C$8,E10)</f>
-        <v>a</v>
+      <c r="E8" t="str">
+        <v>library</v>
+      </c>
+      <c r="F8" t="str">
+        <v>randomSeed</v>
+      </c>
+      <c r="G8" t="str">
+        <v>setPort</v>
+      </c>
+      <c r="H8" t="str">
+        <v>hopen</v>
+      </c>
+      <c r="I8" t="str">
+        <v>bus.client</v>
+      </c>
+      <c r="J8" t="str">
+        <v>tick.cdb</v>
+      </c>
+      <c r="K8" t="str">
+        <v>heartbeat.client</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E9" t="str">
+        <v>arg</v>
+      </c>
+      <c r="F9" t="str">
+        <v>enlist `setPort!enlist "%basePort% + 5"</v>
+      </c>
+      <c r="G9" t="str">
+        <v/>
+      </c>
+      <c r="H9" t="str">
+        <v/>
+      </c>
+      <c r="I9" t="str">
+        <v/>
+      </c>
+      <c r="J9" t="str">
+        <v/>
+      </c>
+      <c r="K9" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E10" t="str">
+        <v>global</v>
+      </c>
+      <c r="F10" t="str">
+        <v>`audit`data`host`instance`basePort!("audit";"data";"localhost";1;25000)</v>
+      </c>
+      <c r="G10" t="str">
+        <v/>
+      </c>
+      <c r="H10" t="str">
+        <v/>
+      </c>
+      <c r="I10" t="str">
+        <v/>
+      </c>
+      <c r="J10" t="str">
+        <v/>
+      </c>
+      <c r="K10" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E11" t="str">
+        <v>local</v>
       </c>
       <c r="F11" t="str">
-        <v>b</v>
+        <v>`$()!()</v>
       </c>
       <c r="G11" t="str">
-        <v>c</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E12">
+        <v/>
+      </c>
+      <c r="H11" t="str">
+        <v/>
+      </c>
+      <c r="I11" t="str">
+        <v/>
+      </c>
+      <c r="J11" t="str">
+        <v/>
+      </c>
+      <c r="K11" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E12" t="str">
+        <v>instance</v>
+      </c>
+      <c r="F12">
         <v>1</v>
       </c>
-      <c r="F12">
-        <v>4</v>
-      </c>
-      <c r="G12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E13">
-        <v>2</v>
+      <c r="G12" t="str">
+        <v/>
+      </c>
+      <c r="H12" t="str">
+        <v/>
+      </c>
+      <c r="I12" t="str">
+        <v/>
+      </c>
+      <c r="J12" t="str">
+        <v/>
+      </c>
+      <c r="K12" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E13" t="str">
+        <v>id</v>
       </c>
       <c r="F13">
-        <v>5</v>
-      </c>
-      <c r="G13">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E14">
-        <v>3</v>
-      </c>
-      <c r="F14">
-        <v>6</v>
-      </c>
-      <c r="G14">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="G13" t="str">
+        <v/>
+      </c>
+      <c r="H13" t="str">
+        <v/>
+      </c>
+      <c r="I13" t="str">
+        <v/>
+      </c>
+      <c r="J13" t="str">
+        <v/>
+      </c>
+      <c r="K13" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E14" t="str">
+        <v>mergeArg</v>
+      </c>
+      <c r="F14" t="str">
+        <v>`audit`basePort`data`host`instance`setPort!("audit";25000;"data";"localhost";1;"%basePort% + 5")</v>
+      </c>
+      <c r="G14" t="str">
+        <v/>
+      </c>
+      <c r="H14" t="str">
+        <v/>
+      </c>
+      <c r="I14" t="str">
+        <v/>
+      </c>
+      <c r="J14" t="str">
+        <v/>
+      </c>
+      <c r="K14" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E15" t="str">
+        <v>host</v>
+      </c>
+      <c r="F15" t="str">
+        <v>localhost</v>
+      </c>
+      <c r="G15" t="str">
+        <v/>
+      </c>
+      <c r="H15" t="str">
+        <v/>
+      </c>
+      <c r="I15" t="str">
+        <v/>
+      </c>
+      <c r="J15" t="str">
+        <v/>
+      </c>
+      <c r="K15" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E16" t="str">
+        <v>port</v>
+      </c>
+      <c r="F16">
+        <v>25005</v>
+      </c>
+      <c r="G16" t="str">
+        <v/>
+      </c>
+      <c r="H16" t="str">
+        <v/>
+      </c>
+      <c r="I16" t="str">
+        <v/>
+      </c>
+      <c r="J16" t="str">
+        <v/>
+      </c>
+      <c r="K16" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E17" t="str">
+        <v>proc</v>
+      </c>
+      <c r="F17" t="str">
+        <v>cdb.0</v>
+      </c>
+      <c r="G17" t="str">
+        <v/>
+      </c>
+      <c r="H17" t="str">
+        <v/>
+      </c>
+      <c r="I17" t="str">
+        <v/>
+      </c>
+      <c r="J17" t="str">
+        <v/>
+      </c>
+      <c r="K17" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E18" t="str">
+        <v>uid</v>
+      </c>
+      <c r="F18" t="str">
+        <v>plant.deepData.mxnet.cdb.0</v>
+      </c>
+      <c r="G18" t="str">
+        <v/>
+      </c>
+      <c r="H18" t="str">
+        <v/>
+      </c>
+      <c r="I18" t="str">
+        <v/>
+      </c>
+      <c r="J18" t="str">
+        <v/>
+      </c>
+      <c r="K18" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E19" t="str">
+        <v>hdb</v>
+      </c>
+      <c r="F19" t="str">
+        <v>data/plant/deepData/mxnet/hdb</v>
+      </c>
+      <c r="G19" t="str">
+        <v/>
+      </c>
+      <c r="H19" t="str">
+        <v/>
+      </c>
+      <c r="I19" t="str">
+        <v/>
+      </c>
+      <c r="J19" t="str">
+        <v/>
+      </c>
+      <c r="K19" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E20" t="str">
+        <v>audit</v>
+      </c>
+      <c r="F20" t="str">
+        <v>audit/plant/deepData/mxnet/cdb/0</v>
+      </c>
+      <c r="G20" t="str">
+        <v/>
+      </c>
+      <c r="H20" t="str">
+        <v/>
+      </c>
+      <c r="I20" t="str">
+        <v/>
+      </c>
+      <c r="J20" t="str">
+        <v/>
+      </c>
+      <c r="K20" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E21" t="str">
+        <v>gData</v>
+      </c>
+      <c r="F21" t="str">
+        <v>data/plant/deepData/mxnet/cdb</v>
+      </c>
+      <c r="G21" t="str">
+        <v/>
+      </c>
+      <c r="H21" t="str">
+        <v/>
+      </c>
+      <c r="I21" t="str">
+        <v/>
+      </c>
+      <c r="J21" t="str">
+        <v/>
+      </c>
+      <c r="K21" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E22" t="str">
+        <v>data</v>
+      </c>
+      <c r="F22" t="str">
+        <v>data/plant/deepData/mxnet/cdb/0</v>
+      </c>
+      <c r="G22" t="str">
+        <v/>
+      </c>
+      <c r="H22" t="str">
+        <v/>
+      </c>
+      <c r="I22" t="str">
+        <v/>
+      </c>
+      <c r="J22" t="str">
+        <v/>
+      </c>
+      <c r="K22" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E23" t="str">
+        <v>gfile</v>
+      </c>
+      <c r="F23" t="str">
+        <v>plant/deepData/mxnet/cdb/global</v>
+      </c>
+      <c r="G23" t="str">
+        <v/>
+      </c>
+      <c r="H23" t="str">
+        <v/>
+      </c>
+      <c r="I23" t="str">
+        <v/>
+      </c>
+      <c r="J23" t="str">
+        <v/>
+      </c>
+      <c r="K23" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E24" t="str">
+        <v>lfile</v>
+      </c>
+      <c r="F24" t="str">
+        <v>plant/deepData/mxnet/cdb/0</v>
+      </c>
+      <c r="G24" t="str">
+        <v/>
+      </c>
+      <c r="H24" t="str">
+        <v/>
+      </c>
+      <c r="I24" t="str">
+        <v/>
+      </c>
+      <c r="J24" t="str">
+        <v/>
+      </c>
+      <c r="K24" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E25" t="str">
+        <v>gcorefile</v>
+      </c>
+      <c r="F25" t="str">
+        <v>C:\q\btick\core\core\mxnet\cdb\global</v>
+      </c>
+      <c r="G25" t="str">
+        <v/>
+      </c>
+      <c r="H25" t="str">
+        <v/>
+      </c>
+      <c r="I25" t="str">
+        <v/>
+      </c>
+      <c r="J25" t="str">
+        <v/>
+      </c>
+      <c r="K25" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E26" t="str">
+        <v>lcorefile</v>
+      </c>
+      <c r="F26" t="str">
+        <v>C:\q\btick\core\core\mxnet\cdb\0</v>
+      </c>
+      <c r="G26" t="str">
+        <v/>
+      </c>
+      <c r="H26" t="str">
+        <v/>
+      </c>
+      <c r="I26" t="str">
+        <v/>
+      </c>
+      <c r="J26" t="str">
+        <v/>
+      </c>
+      <c r="K26" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>